<commit_message>
update V+ to USB
</commit_message>
<xml_diff>
--- a/BathymetryLab/Microcontroller/SensorPartsList.xlsx
+++ b/BathymetryLab/Microcontroller/SensorPartsList.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Robert\Documents\projects\inProgress\PublicSensors\BathymetryLab\BathymetryLab\Microcontroller\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A1CD1DD0-CB92-4AD8-AC13-BBFB78E0E226}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{614C3459-E035-4304-BA8F-E77F7F206876}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="23052" yWindow="5808" windowWidth="18612" windowHeight="18684" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2160" yWindow="0" windowWidth="14805" windowHeight="12360" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="materials + cost" sheetId="1" r:id="rId1"/>
@@ -526,15 +526,15 @@
   <dimension ref="A1:Z18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E32" sqref="E32"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="36.21875" customWidth="1"/>
+    <col min="1" max="1" width="36.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -544,7 +544,7 @@
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
     </row>
-    <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>5</v>
       </c>
@@ -554,7 +554,7 @@
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
     </row>
-    <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -562,7 +562,7 @@
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
     </row>
-    <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
@@ -570,7 +570,7 @@
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
     </row>
-    <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>0</v>
       </c>
@@ -590,7 +590,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>7</v>
       </c>
@@ -611,7 +611,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
@@ -632,7 +632,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>11</v>
       </c>
@@ -651,7 +651,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
         <v>1</v>
       </c>
@@ -670,7 +670,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>9</v>
       </c>
@@ -691,7 +691,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:26" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
@@ -699,7 +699,7 @@
       <c r="E11" s="4"/>
       <c r="F11" s="4"/>
     </row>
-    <row r="12" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A12" s="4"/>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
@@ -707,7 +707,7 @@
       <c r="E12" s="4"/>
       <c r="F12" s="4"/>
     </row>
-    <row r="13" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A13" s="4"/>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
@@ -715,7 +715,7 @@
       <c r="E13" s="4"/>
       <c r="F13" s="4"/>
     </row>
-    <row r="14" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A14" s="7" t="s">
         <v>20</v>
       </c>
@@ -748,17 +748,17 @@
       <c r="Y14" s="10"/>
       <c r="Z14" s="10"/>
     </row>
-    <row r="16" spans="1:26" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:26" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="17" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="18" spans="1:1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" ht="12.75" x14ac:dyDescent="0.2">
       <c r="A18" s="11" t="s">
         <v>17</v>
       </c>

</xml_diff>